<commit_message>
last push of the morning
</commit_message>
<xml_diff>
--- a/to-do-list.xlsx
+++ b/to-do-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="143">
   <si>
     <t xml:space="preserve">TO DO LIST EXAMEN S3 – 16 décembre 2025 (PART I)</t>
   </si>
@@ -91,6 +91,9 @@
     <t xml:space="preserve">Zones</t>
   </si>
   <si>
+    <t xml:space="preserve">(utilisation à prévoir)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Colis</t>
   </si>
   <si>
@@ -229,9 +232,6 @@
     <t xml:space="preserve">4.</t>
   </si>
   <si>
-    <t xml:space="preserve">wip</t>
-  </si>
-  <si>
     <t xml:space="preserve">Données de test</t>
   </si>
   <si>
@@ -241,9 +241,6 @@
     <t xml:space="preserve">5.</t>
   </si>
   <si>
-    <t xml:space="preserve">not started</t>
-  </si>
-  <si>
     <t xml:space="preserve">Accueil</t>
   </si>
   <si>
@@ -253,6 +250,12 @@
     <t xml:space="preserve">Design</t>
   </si>
   <si>
+    <t xml:space="preserve">Landing Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fonctions</t>
   </si>
   <si>
@@ -268,34 +271,184 @@
     <t xml:space="preserve">Affectation</t>
   </si>
   <si>
+    <t xml:space="preserve">Views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colis disponibles : idColis not in Livraison</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trigger</t>
   </si>
   <si>
     <t xml:space="preserve">On insert into Livraison : insert into LivraisonStatut (en attente)</t>
   </si>
   <si>
+    <t xml:space="preserve">Procédure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nouvelle livraison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vérifier que le colis est encore disponible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vérifier les paramètres entrés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transaction : insert into affectation → insert into livraison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulaire de création :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloc affectation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choix du chauffeur : liste déroulante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choix du véhicule : liste déroulante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloc colis : tableau de sélection de colis disponibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloc bénéfice : coût véhicule, livreur, prix par kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">créer(idVehicule, idLivreur, coutVehicule, coutLivreur, idColis, prixKg, dateLivraison) → appel de la procédure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LivraisonController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage du formulaire : chargement des données (liste véhicules, chauffeur, colis)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enregistrement : fonction créer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gestion statut livraison</t>
   </si>
   <si>
-    <t xml:space="preserve">Procédure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AcheverLivraison (idLivraison)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Vérifier que la livraison est en cours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Récupérer les informations de la livraison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Transaction </t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Insert into Paiements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- change LivraisonStatut (livré)</t>
+    <t xml:space="preserve">Statut actuel des livraisons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmer livraison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Récupérer le statut actuel de la livraison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Vérifier que la livraison est bien en attente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Vérifier les informations du colis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Récupérer les informations de paiement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Transaction : insert into Paiements → update status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tableau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste des colis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statut de la livraison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si en attente → Confirmer ou Supprimer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achever livraison → appel de la procedure Confirmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annuler livraison → appel de la procedure Annuler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StatutController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefices par période</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefices par mois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefices par annee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulaire de filtre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mois (1 – 12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour (1 – 31)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tableau résultat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ligne total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getBeneficesParPeriode → utilise les views selon la sélection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculerTotaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BeneficeController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefices détaillés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéfices détaillés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloc récapitulatif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total livraisons livrés ou annulés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiffre d’affaires total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coûts totaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bénéfice Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marge en %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tableau détaillé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getBeneficesDetailles</t>
   </si>
 </sst>
 </file>
@@ -377,7 +530,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -391,6 +544,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -620,10 +777,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O140"/>
+  <dimension ref="A1:O201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K127" activeCellId="0" sqref="K127"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="113" zoomScaleNormal="113" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B202" activeCellId="0" sqref="B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -853,7 +1010,9 @@
         <v>22</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -871,7 +1030,7 @@
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -889,7 +1048,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -907,7 +1066,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -918,11 +1077,14 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -943,13 +1105,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -963,26 +1125,26 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,7 +1165,7 @@
       <c r="A27" s="2"/>
       <c r="C27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1012,16 +1174,16 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1031,7 +1193,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="3"/>
       <c r="F29" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1041,7 +1203,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="3"/>
       <c r="F30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1053,285 +1215,288 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="3"/>
       <c r="E33" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F34" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F44" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F46" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F47" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F48" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F55" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F61" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F62" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F63" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="C71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F74" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F75" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>70</v>
@@ -1343,35 +1508,35 @@
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2"/>
       <c r="B78" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>71</v>
@@ -1379,24 +1544,24 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,10 +1569,10 @@
         <v>72</v>
       </c>
       <c r="C84" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
@@ -1415,214 +1580,725 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D85" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D86" s="1" t="s">
         <v>75</v>
       </c>
     </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D88" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D91" s="1" t="s">
+      <c r="B88" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>77</v>
       </c>
     </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D89" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D90" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D93" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D94" s="1" t="s">
-        <v>78</v>
+      <c r="E94" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F95" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F96" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F97" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
+      <c r="F98" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D99" s="1" t="s">
-        <v>75</v>
+      <c r="F99" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E100" s="1" t="s">
-        <v>80</v>
+      <c r="F100" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F101" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F102" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F103" s="1" t="s">
-        <v>22</v>
+      <c r="E103" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F104" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F105" s="1" t="s">
-        <v>23</v>
+      <c r="E105" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F106" s="1" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F107" s="1" t="s">
-        <v>21</v>
+      <c r="E107" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F108" s="1" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E109" s="1" t="s">
-        <v>82</v>
+      <c r="G109" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F110" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D112" s="1" t="s">
-        <v>76</v>
+      <c r="G110" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G111" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D113" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D114" s="1" t="s">
-        <v>77</v>
+      <c r="B114" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F115" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D116" s="1" t="s">
+      <c r="F116" s="0"/>
+      <c r="G116" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F117" s="0"/>
+      <c r="G117" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F118" s="0"/>
+      <c r="G118" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F119" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F120" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D122" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E118" s="2"/>
-      <c r="F118" s="2"/>
-      <c r="G118" s="2"/>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D119" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E120" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F121" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F122" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F123" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F124" s="1" t="s">
-        <v>25</v>
+      <c r="B123" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F125" s="1" t="s">
-        <v>26</v>
+      <c r="D125" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E126" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F127" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G128" s="1" t="s">
+      <c r="F128" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D131" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E132" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F133" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F134" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F135" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F136" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F137" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E138" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E140" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G129" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G130" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H131" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H132" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D134" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D137" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D140" s="1" t="s">
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B141" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G142" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G143" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G144" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G145" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G146" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D148" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F150" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F151" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F152" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D154" s="1" t="s">
         <v>78</v>
       </c>
     </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D158" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B159" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D162" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E163" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B164" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B165" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B166" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D168" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F170" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F171" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F172" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B173" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B174" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D176" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B177" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B178" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D180" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B181" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E183" s="2"/>
+      <c r="F183" s="2"/>
+      <c r="G183" s="2"/>
+    </row>
+    <row r="184" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="3"/>
+      <c r="B184" s="3"/>
+      <c r="C184" s="3"/>
+      <c r="D184" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E184" s="3"/>
+      <c r="F184" s="3"/>
+      <c r="G184" s="3"/>
+      <c r="H184" s="3"/>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E185" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B186" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D188" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B189" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F190" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F191" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F192" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F193" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F194" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B195" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D197" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B198" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D200" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B201" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C4:C8 C10:C75 C77:C1048576 C1 B2:B3">
+  <conditionalFormatting sqref="C4:C8 C10:C75 C1 B2:B3 C77:C1048576">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="ok" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("ok",B1)))</formula>
     </cfRule>
@@ -1644,7 +2320,7 @@
       <formula>NOT(ISERROR(SEARCH("wip",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C75 C77:C1048576 C1 B2:B3">
+  <conditionalFormatting sqref="C4:C75 C1 B2:B3 C77:C1048576">
     <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="not started" dxfId="3">
       <formula>NOT(ISERROR(SEARCH("not started",B1)))</formula>
     </cfRule>
@@ -1653,8 +2329,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>